<commit_message>
cambio del historico y del 31b
</commit_message>
<xml_diff>
--- a/xlsx/a69_f31_bUPPachuca.xlsx
+++ b/xlsx/a69_f31_bUPPachuca.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
   <si>
     <t>46637</t>
   </si>
@@ -149,15 +149,6 @@
     <t>Estado de Situación Financiera</t>
   </si>
   <si>
-    <t>https://s-finanzas.hidalgo.gob.mx/pag/48Rubros.html                                                                                                                          http://transparencia.hidalgo.gob.mx/descargables/dependencias/finanzasadmon/16edofinanciero.pdf</t>
-  </si>
-  <si>
-    <t>https://s-finanzas.hidalgo.gob.mx/pag/48Rubros.html                                                                                                                                                                                                                                                http://transparencia.hidalgo.gob.mx/descargables/dependencias/finanzasadmon/16edof</t>
-  </si>
-  <si>
-    <t>https://s-finanzas.hidalgo.gob.mx/pag/48Rubros.html                                                                                                                                   http://transparencia.hidalgo.gob.mx/descargables/dependencias/finanzasadmon/16edofinanciero.pdf</t>
-  </si>
-  <si>
     <t>Presupuesto Anual de Egresos Convenio</t>
   </si>
   <si>
@@ -171,6 +162,9 @@
   </si>
   <si>
     <t>https://www.upp.edu.mx/leygralcontabilidad/mc/01-edosfin/2022/a_marzo_2022/estado-de-situacion-financiera.pdf</t>
+  </si>
+  <si>
+    <t>https://finanzas.hidalgo.gob.mx/transparenciafinanzas/EdosFin</t>
   </si>
 </sst>
 </file>
@@ -262,7 +256,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -276,20 +270,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -563,7 +558,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -573,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD46"/>
+    <sheetView tabSelected="1" topLeftCell="G2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,33 +593,33 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="5" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="5" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
     </row>
     <row r="3" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7" t="s">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
       <c r="G3" s="9" t="s">
         <v>6</v>
       </c>
@@ -702,19 +697,19 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -764,14 +759,14 @@
       <c r="D8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="5" t="s">
         <v>42</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>41</v>
@@ -797,14 +792,14 @@
       <c r="D9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>46</v>
+      <c r="E9" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" s="4" t="s">
         <v>44</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>40</v>
@@ -830,14 +825,14 @@
       <c r="D10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="11" t="s">
         <v>48</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>40</v>
@@ -866,14 +861,15 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G8" r:id="rId1" display="https://s-finanzas.hidalgo.gob.mx/pag/48Rubros.html "/>
-    <hyperlink ref="G9" r:id="rId2" display="https://s-finanzas.hidalgo.gob.mx/pag/48Rubros.html "/>
-    <hyperlink ref="G10" r:id="rId3" display="https://s-finanzas.hidalgo.gob.mx/pag/48Rubros.html "/>
-    <hyperlink ref="F9" r:id="rId4"/>
-    <hyperlink ref="F10" r:id="rId5"/>
-    <hyperlink ref="F8" r:id="rId6"/>
+    <hyperlink ref="F9" r:id="rId1"/>
+    <hyperlink ref="F10" r:id="rId2"/>
+    <hyperlink ref="F8" r:id="rId3"/>
+    <hyperlink ref="G8" r:id="rId4"/>
+    <hyperlink ref="G9" r:id="rId5"/>
+    <hyperlink ref="G10" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -881,7 +877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>